<commit_message>
Added support for Knee of Spectral plot
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/scalar_metric_results.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/scalar_metric_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Shepard Goodness</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Stress</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -462,30 +467,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.791853570968416</v>
+        <v>0.7801047205449106</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8311670840546946</v>
+        <v>0.8238262518122003</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2339968774395003</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>[[ 1.         -0.50182497  0.91884202 ... -0.27671161 -0.11469325
-   0.7955566 ]
- [-0.50182497  1.         -0.45300939 ...  0.25732629 -0.31753919
-  -0.37844807]
- [ 0.91884202 -0.45300939  1.         ... -0.27886236 -0.15105878
-   0.85590914]
- ...
- [-0.27671161  0.25732629 -0.27886236 ...  1.          0.16373369
-   0.11704076]
- [-0.11469325 -0.31753919 -0.15105878 ...  0.16373369  1.
-  -0.21615053]
- [ 0.7955566  -0.37844807  0.85590914 ...  0.11704076 -0.21615053
-   1.        ]]</t>
-        </is>
+        <v>0.2320452771272443</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.6553455820268151</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.3681470042108818</v>
       </c>
     </row>
     <row r="3">
@@ -495,30 +489,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7025566381919935</v>
+        <v>0.6963833204001391</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7471366643614195</v>
+        <v>0.7480795429333351</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3592546583850931</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.24549232  0.26456086 ...  0.12470318 -0.13802661
-   0.11871252]
- [ 0.24549232  1.          0.3451146  ...  0.38811655 -0.12267187
-   0.04122   ]
- [ 0.26456086  0.3451146   1.         ...  0.02567973  0.33571444
-  -0.36488979]
- ...
- [ 0.12470318  0.38811655  0.02567973 ...  1.         -0.4129284
-   0.52521889]
- [-0.13802661 -0.12267187  0.33571444 ... -0.4129284   1.
-  -0.93836754]
- [ 0.11871252  0.04122    -0.36488979 ...  0.52521889 -0.93836754
-   1.        ]]</t>
-        </is>
+        <v>0.3637267080745342</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.2545431206831705</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.5096978881398675</v>
       </c>
     </row>
     <row r="4">
@@ -528,30 +511,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.7316378787571052</v>
+        <v>0.7354680641490043</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8429543990282949</v>
+        <v>0.8389617838099908</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7566860336186633</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.33781563 -0.00476972 ...  0.11218403 -0.11088928
-   0.01292562]
- [ 0.33781563  1.          0.23666436 ...  0.08495347 -0.10359091
-  -0.03014465]
- [-0.00476972  0.23666436  1.         ... -0.01582472 -0.12998506
-  -0.11488373]
- ...
- [ 0.11218403  0.08495347 -0.01582472 ...  1.         -0.21444067
-   0.49651923]
- [-0.11088928 -0.10359091 -0.12998506 ... -0.21444067  1.
-   0.61192412]
- [ 0.01292562 -0.03014465 -0.11488373 ...  0.49651923  0.61192412
-   1.        ]]</t>
-        </is>
+        <v>0.754690202687719</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1010465285793719</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.6020072456588343</v>
       </c>
     </row>
     <row r="5">
@@ -561,30 +533,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6809725409054832</v>
+        <v>0.6801473389811592</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8109415400867011</v>
+        <v>0.8164299325198088</v>
       </c>
       <c r="D5" t="n">
-        <v>0.604543564150551</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.09173335  0.69329634 ... -0.09052683 -0.07943836
-  -0.09550172]
- [ 0.09173335  1.         -0.03944938 ... -0.01097452 -0.06798695
-   0.00686978]
- [ 0.69329634 -0.03944938  1.         ... -0.06098899 -0.07535782
-  -0.05455584]
- ...
- [-0.09052683 -0.01097452 -0.06098899 ...  1.          0.89408391
-   0.94164208]
- [-0.07943836 -0.06798695 -0.07535782 ...  0.89408391  1.
-   0.75073688]
- [-0.09550172  0.00686978 -0.05455584 ...  0.94164208  0.75073688
-   1.        ]]</t>
-        </is>
+        <v>0.5982012892493241</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.04631739834967147</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.5783779263472448</v>
       </c>
     </row>
     <row r="6">
@@ -594,30 +555,19 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.6095806049267227</v>
+        <v>0.6003302547502734</v>
       </c>
       <c r="C6" t="n">
-        <v>0.6337949970550532</v>
+        <v>0.6585967699625324</v>
       </c>
       <c r="D6" t="n">
-        <v>0.3558201058201058</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.69791144  0.85282838 ...  0.08865007 -0.01773375
-  -0.091858  ]
- [ 0.69791144  1.          0.75517582 ...  0.14385215  0.00401197
-  -0.09526049]
- [ 0.85282838  0.75517582  1.         ...  0.13168817  0.0045261
-  -0.09587751]
- ...
- [ 0.08865007  0.14385215  0.13168817 ...  1.          0.2911623
-  -0.26338402]
- [-0.01773375  0.00401197  0.0045261  ...  0.2911623   1.
-   0.73657104]
- [-0.091858   -0.09526049 -0.09587751 ... -0.26338402  0.73657104
-   1.        ]]</t>
-        </is>
+        <v>0.3529100529100529</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.05877359773775075</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.6066793309427496</v>
       </c>
     </row>
     <row r="7">
@@ -627,30 +577,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.789025167449765</v>
+        <v>0.8054873815633088</v>
       </c>
       <c r="C7" t="n">
-        <v>0.8808858037033335</v>
+        <v>0.881254651382363</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4653769841269841</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>[[ 1.00000000e+00  9.90260914e-01  3.60927330e-01 ...  5.36696102e-02
-   3.22635428e-02  1.37592595e-01]
- [ 9.90260914e-01  1.00000000e+00  3.43584668e-01 ...  2.73458007e-02
-  -2.33820522e-04  1.31355825e-01]
- [ 3.60927330e-01  3.43584668e-01  1.00000000e+00 ... -1.36547821e-01
-  -9.45434926e-02 -2.88103486e-01]
- ...
- [ 5.36696102e-02  2.73458007e-02 -1.36547821e-01 ...  1.00000000e+00
-   9.82447743e-01  7.62548219e-01]
- [ 3.22635428e-02 -2.33820522e-04 -9.45434926e-02 ...  9.82447743e-01
-   1.00000000e+00  6.64804735e-01]
- [ 1.37592595e-01  1.31355825e-01 -2.88103486e-01 ...  7.62548219e-01
-   6.64804735e-01  1.00000000e+00]]</t>
-        </is>
+        <v>0.4763888888888889</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.3844378513214239</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.4737223784383462</v>
       </c>
     </row>
     <row r="8">
@@ -660,30 +599,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.731012800790084</v>
+        <v>0.7296140813050569</v>
       </c>
       <c r="C8" t="n">
-        <v>0.6495577721283236</v>
+        <v>0.6456888777023624</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2302622152170798</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.87486936 -0.70086606 ...  0.5771237  -0.23330727
-   0.21315078]
- [ 0.87486936  1.         -0.62284048 ...  0.53040419 -0.18122831
-   0.16975495]
- [-0.70086606 -0.62284048  1.         ... -0.48469082  0.17316819
-  -0.1447985 ]
- ...
- [ 0.5771237   0.53040419 -0.48469082 ...  1.          0.28774563
-   0.07322826]
- [-0.23330727 -0.18122831  0.17316819 ...  0.28774563  1.
-  -0.7525101 ]
- [ 0.21315078  0.16975495 -0.1447985  ...  0.07322826 -0.7525101
-   1.        ]]</t>
-        </is>
+        <v>0.2359936953718297</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2556600436183515</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.5171676536893606</v>
       </c>
     </row>
     <row r="9">
@@ -693,30 +621,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.7313135718865882</v>
+        <v>0.7330949384052193</v>
       </c>
       <c r="C9" t="n">
-        <v>0.7580264971212795</v>
+        <v>0.7508288204540134</v>
       </c>
       <c r="D9" t="n">
-        <v>0.2469890109890109</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.00647568  0.34009777 ...  0.19819035 -0.285525
-   0.31461278]
- [ 0.00647568  1.          0.24606249 ...  0.05797448 -0.10018054
-   0.08334466]
- [ 0.34009777  0.24606249  1.         ...  0.36107631 -0.25283729
-   0.28973795]
- ...
- [ 0.19819035  0.05797448  0.36107631 ...  1.          0.01478296
-   0.55990405]
- [-0.285525   -0.10018054 -0.25283729 ...  0.01478296  1.
-  -0.72479712]
- [ 0.31461278  0.08334466  0.28973795 ...  0.55990405 -0.72479712
-   1.        ]]</t>
-        </is>
+        <v>0.2461978021978022</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.3575377327384222</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4669359961636719</v>
       </c>
     </row>
     <row r="10">
@@ -726,30 +643,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.7571217002023292</v>
+        <v>0.7762348292947155</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8239804202711529</v>
+        <v>0.8329187019069924</v>
       </c>
       <c r="D10" t="n">
-        <v>0.3734285714285714</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.21055346 -0.30185171 ... -0.60282867  0.47829819
-  -0.51010657]
- [ 0.21055346  1.          0.73101407 ... -0.35531748  0.42706574
-  -0.0219184 ]
- [-0.30185171  0.73101407  1.         ... -0.05389376  0.13157509
-   0.18840818]
- ...
- [-0.60282867 -0.35531748 -0.05389376 ...  1.         -0.30042769
-   0.85321867]
- [ 0.47829819  0.42706574  0.13157509 ... -0.30042769  1.
-  -0.39717126]
- [-0.51010657 -0.0219184   0.18840818 ...  0.85321867 -0.39717126
-   1.        ]]</t>
-        </is>
+        <v>0.4031428571428571</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.4130199962296499</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.4537020418065079</v>
       </c>
     </row>
     <row r="11">
@@ -759,30 +665,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6119822767779282</v>
+        <v>0.6082935377511274</v>
       </c>
       <c r="C11" t="n">
-        <v>0.6140174574567924</v>
+        <v>0.6226620960575382</v>
       </c>
       <c r="D11" t="n">
-        <v>0.8605645851154833</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.10026829  0.42273501 ...  0.15322599 -0.0890674
-  -0.06244378]
- [ 0.10026829  1.          0.02990535 ...  0.04045102 -0.09472506
-  -0.08578368]
- [ 0.42273501  0.02990535  1.         ...  0.06155976 -0.00445839
-   0.01492026]
- ...
- [ 0.15322599  0.04045102  0.06155976 ...  1.         -0.94856685
-  -0.92488746]
- [-0.0890674  -0.09472506 -0.00445839 ... -0.94856685  1.
-   0.98423343]
- [-0.06244378 -0.08578368  0.01492026 ... -0.92488746  0.98423343
-   1.        ]]</t>
-        </is>
+        <v>0.8740804106073568</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.02186882263165332</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.601405077772967</v>
       </c>
     </row>
     <row r="12">
@@ -792,30 +687,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.747481707551769</v>
+        <v>0.7356362468192377</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8617739834227298</v>
+        <v>0.8511145799574147</v>
       </c>
       <c r="D12" t="n">
-        <v>0.7999503213587108</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.12286999 -0.03485827 ...  0.17513147  0.11625475
-   0.25367696]
- [ 0.12286999  1.          0.66376839 ...  0.21117464  0.02624959
-   0.27365945]
- [-0.03485827  0.66376839  1.         ... -0.01636226 -0.06963605
-  -0.0898254 ]
- ...
- [ 0.17513147  0.21117464 -0.01636226 ...  1.          0.9081234
-   0.6804002 ]
- [ 0.11625475  0.02624959 -0.06963605 ...  0.9081234   1.
-   0.39485396]
- [ 0.25367696  0.27365945 -0.0898254  ...  0.6804002   0.39485396
-   1.        ]]</t>
-        </is>
+        <v>0.8179588288260315</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.1807333835319507</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.5464286012668539</v>
       </c>
     </row>
     <row r="13">
@@ -825,30 +709,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.672797502941803</v>
+        <v>0.6712767999370041</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6257754091279912</v>
+        <v>0.6388792931516981</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8933357644270217</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.57648539  0.1648354  ... -0.0889947  -0.09955304
-  -0.078086  ]
- [ 0.57648539  1.          0.22523944 ... -0.11723348 -0.12156771
-  -0.10425133]
- [ 0.1648354   0.22523944  1.         ...  0.00787041  0.01685657
-   0.02219125]
- ...
- [-0.0889947  -0.11723348  0.00787041 ...  1.          0.94871016
-   0.95314844]
- [-0.09955304 -0.12156771  0.01685657 ...  0.94871016  1.
-   0.99887484]
- [-0.078086   -0.10425133  0.02219125 ...  0.95314844  0.99887484
-   1.        ]]</t>
-        </is>
+        <v>0.8947032546266752</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.107127972599875</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.5798696577192061</v>
       </c>
     </row>
     <row r="14">
@@ -858,30 +731,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.8451277568632094</v>
+        <v>0.8960027442390135</v>
       </c>
       <c r="C14" t="n">
-        <v>0.9235819980706746</v>
+        <v>0.9597551080108795</v>
       </c>
       <c r="D14" t="n">
-        <v>0.8962848297213623</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>[[ 1.         -0.20660445 -0.17103892 ...  0.68614403  0.52252417
-   0.16271903]
- [-0.20660445  1.          0.42527491 ... -0.51511114 -0.54548226
-  -0.04490096]
- [-0.17103892  0.42527491  1.         ... -0.25447764 -0.5095316
-  -0.12922859]
- ...
- [ 0.68614403 -0.51511114 -0.25447764 ...  1.          0.85082601
-   0.26212195]
- [ 0.52252417 -0.54548226 -0.5095316  ...  0.85082601  1.
-   0.60746778]
- [ 0.16271903 -0.04490096 -0.12922859 ...  0.26212195  0.60746778
-   1.        ]]</t>
-        </is>
+        <v>0.8993808049535603</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.4917461058793112</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.4113595306608349</v>
       </c>
     </row>
     <row r="15">
@@ -891,30 +753,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.8220650849132076</v>
+        <v>0.8454515192027876</v>
       </c>
       <c r="C15" t="n">
-        <v>0.796636760465828</v>
+        <v>0.8289137122883882</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4989310009718173</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.92333962 -0.86589279 ...  0.71298781  0.79263332
-   0.62170135]
- [ 0.92333962  1.         -0.88282406 ...  0.70947142  0.78015381
-   0.63427023]
- [-0.86589279 -0.88282406  1.         ... -0.71687986 -0.7757767
-  -0.54391379]
- ...
- [ 0.71298781  0.70947142 -0.71687986 ...  1.          0.96289606
-   0.64949025]
- [ 0.79263332  0.78015381 -0.7757767  ...  0.96289606  1.
-   0.75741389]
- [ 0.62170135  0.63427023 -0.54391379 ...  0.64949025  0.75741389
-   1.        ]]</t>
-        </is>
+        <v>0.5378036929057336</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.6810948176154288</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.3525731832739853</v>
       </c>
     </row>
     <row r="16">
@@ -924,30 +775,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.4095969518912964</v>
+        <v>0.4438229893499817</v>
       </c>
       <c r="C16" t="n">
-        <v>0.9957620271759089</v>
+        <v>0.9964579507895703</v>
       </c>
       <c r="D16" t="n">
         <v>0.9142857142857143</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.99763653  0.99547231 ... -0.88207529 -0.88207529
-  -0.88207529]
- [ 0.99763653  1.          0.99830904 ... -0.88165348 -0.88165348
-  -0.88165348]
- [ 0.99547231  0.99830904  1.         ... -0.88050601 -0.88050601
-  -0.88050601]
- ...
- [-0.88207529 -0.88165348 -0.88050601 ...  1.          1.
-   1.        ]
- [-0.88207529 -0.88165348 -0.88050601 ...  1.          1.
-   1.        ]
- [-0.88207529 -0.88165348 -0.88050601 ...  1.          1.
-   1.        ]]</t>
-        </is>
+      <c r="E16" t="n">
+        <v>0.8975655179809208</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.04770904438704689</v>
       </c>
     </row>
     <row r="17">
@@ -957,30 +797,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.6553097495317111</v>
+        <v>0.6551482235628507</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6814475302739971</v>
+        <v>0.6791075402322397</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9423648523128367</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.04511237  0.04599284 ... -0.08326399 -0.04021133
-  -0.07486222]
- [ 0.04511237  1.         -0.24269883 ...  0.12958771  0.11322556
-   0.03656812]
- [ 0.04599284 -0.24269883  1.         ...  0.07480351  0.13569995
-   0.10970974]
- ...
- [-0.08326399  0.12958771  0.07480351 ...  1.          0.8870993
-   0.69918294]
- [-0.04021133  0.11322556  0.13569995 ...  0.8870993   1.
-   0.43974347]
- [-0.07486222  0.03656812  0.10970974 ...  0.69918294  0.43974347
-   1.        ]]</t>
-        </is>
+        <v>0.9410644621958018</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.1056823296212619</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.5921076998944733</v>
       </c>
     </row>
     <row r="18">
@@ -990,30 +819,19 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.5583929784324968</v>
+        <v>0.5603062945082087</v>
       </c>
       <c r="C18" t="n">
-        <v>0.545522827897635</v>
+        <v>0.543901081937513</v>
       </c>
       <c r="D18" t="n">
-        <v>0.6316483516483518</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>[[ 1.          0.01180687  0.06936285 ... -0.00652083  0.03011205
-  -0.0113662 ]
- [ 0.01180687  1.         -0.02402719 ... -0.01327369 -0.02364934
-  -0.0189571 ]
- [ 0.06936285 -0.02402719  1.         ... -0.0178282   0.01262328
-  -0.01688214]
- ...
- [-0.00652083 -0.01327369 -0.0178282  ...  1.          0.41408837
-   0.60130657]
- [ 0.03011205 -0.02364934  0.01262328 ...  0.41408837  1.
-  -0.28650244]
- [-0.0113662  -0.0189571  -0.01688214 ...  0.60130657 -0.28650244
-   1.        ]]</t>
-        </is>
+        <v>0.618065934065934</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.0223717291107003</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.6253724273357325</v>
       </c>
     </row>
     <row r="19">
@@ -1023,30 +841,19 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.7600161515970825</v>
+        <v>0.7719858008503608</v>
       </c>
       <c r="C19" t="n">
-        <v>0.763859625967009</v>
+        <v>0.815857903346805</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8486088947477971</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>[[ 1.         -0.04498195 -0.53616893 ... -0.34228359  0.04642406
-   0.22022922]
- [-0.04498195  1.          0.38683835 ... -0.01541468  0.12432546
-   0.0553033 ]
- [-0.53616893  0.38683835  1.         ...  0.22580175  0.18310046
-  -0.08267467]
- ...
- [-0.34228359 -0.01541468  0.22580175 ...  1.         -0.09990441
-   0.02101653]
- [ 0.04642406  0.12432546  0.18310046 ... -0.09990441  1.
-   0.86230408]
- [ 0.22022922  0.0553033  -0.08267467 ...  0.02101653  0.86230408
-   1.        ]]</t>
-        </is>
+        <v>0.841809477554985</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.2251216530445644</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.5448785226584123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>